<commit_message>
重調 a200, a300 作法
</commit_message>
<xml_diff>
--- a/output7/【河洛文讀注音-閩拼調號】《定風波》.xlsx
+++ b/output7/【河洛文讀注音-閩拼調號】《定風波》.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Piau-Im\output7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC02EBFE-19B7-4497-8F61-6092D06DF8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AD26D85-19FC-4E7C-B5C2-D4C8A628200A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{25A76161-EFED-4AC8-8EAA-A42737AE1909}"/>
   </bookViews>
   <sheets>
     <sheet name="env" sheetId="8" r:id="rId1"/>
-    <sheet name="人工標音字庫" sheetId="330" r:id="rId2"/>
-    <sheet name="標音字庫" sheetId="329" r:id="rId3"/>
-    <sheet name="缺字表" sheetId="328" r:id="rId4"/>
+    <sheet name="人工標音字庫" sheetId="336" r:id="rId2"/>
+    <sheet name="標音字庫" sheetId="335" r:id="rId3"/>
+    <sheet name="缺字表" sheetId="334" r:id="rId4"/>
     <sheet name="漢字注音" sheetId="9" r:id="rId5"/>
     <sheet name="漢字注音 (白話音)" sheetId="279" r:id="rId6"/>
     <sheet name="漢字注音 (2)" sheetId="275" r:id="rId7"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3759" uniqueCount="1619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3846" uniqueCount="1619">
   <si>
     <t>Key</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -5545,9 +5545,6 @@
     <t>Tánn</t>
   </si>
   <si>
-    <t>(57, 18)</t>
-  </si>
-  <si>
     <t>(5, 14); (5, 16)</t>
   </si>
   <si>
@@ -5558,6 +5555,9 @@
   </si>
   <si>
     <t>(21, 18)</t>
+  </si>
+  <si>
+    <t>(57, 18); (33, 18)</t>
   </si>
 </sst>
 </file>
@@ -5996,7 +5996,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -6198,13 +6198,10 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -15235,7 +15232,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66716CFE-44BF-4E4D-9CD1-A5C008FE7600}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81B78BD-7336-4F07-A325-77FF06BA174E}">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15365,7 +15362,7 @@
         <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -15435,7 +15432,7 @@
         <v>1596</v>
       </c>
       <c r="D14" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -15463,7 +15460,7 @@
         <v>1179</v>
       </c>
       <c r="D16" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -15477,7 +15474,7 @@
         <v>1595</v>
       </c>
       <c r="D17" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -15585,10 +15582,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7206F1-181A-4945-A97D-CB8FCAC48960}">
-  <dimension ref="A1:D66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423522E3-30B8-413C-AE61-FCF0512DB4FC}">
+  <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
@@ -16510,10 +16507,318 @@
         <v>334</v>
       </c>
       <c r="C66" t="s">
-        <v>499</v>
+        <v>334</v>
       </c>
       <c r="D66" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>164</v>
+      </c>
+      <c r="B67" t="s">
+        <v>57</v>
+      </c>
+      <c r="C67" t="s">
+        <v>57</v>
+      </c>
+      <c r="D67" t="s">
         <v>1614</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D68" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>167</v>
+      </c>
+      <c r="B69" t="s">
+        <v>386</v>
+      </c>
+      <c r="C69" t="s">
+        <v>386</v>
+      </c>
+      <c r="D69" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" t="s">
+        <v>395</v>
+      </c>
+      <c r="C70" t="s">
+        <v>395</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>222</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>116</v>
+      </c>
+      <c r="B72" t="s">
+        <v>346</v>
+      </c>
+      <c r="C72" t="s">
+        <v>346</v>
+      </c>
+      <c r="D72" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D73" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1552</v>
+      </c>
+      <c r="D74" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>84</v>
+      </c>
+      <c r="B75" t="s">
+        <v>316</v>
+      </c>
+      <c r="C75" t="s">
+        <v>316</v>
+      </c>
+      <c r="D75" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>291</v>
+      </c>
+      <c r="B76" t="s">
+        <v>62</v>
+      </c>
+      <c r="C76" t="s">
+        <v>62</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>199</v>
+      </c>
+      <c r="B77" t="s">
+        <v>359</v>
+      </c>
+      <c r="C77" t="s">
+        <v>359</v>
+      </c>
+      <c r="D77" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>199</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1596</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1596</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D79" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>185</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>185</v>
+      </c>
+      <c r="B81" t="s">
+        <v>353</v>
+      </c>
+      <c r="C81" t="s">
+        <v>353</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D82" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1536</v>
+      </c>
+      <c r="D83" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>210</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D84" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D85" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B86" t="s">
+        <v>380</v>
+      </c>
+      <c r="C86" t="s">
+        <v>380</v>
+      </c>
+      <c r="D86" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>105</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1267</v>
       </c>
     </row>
   </sheetData>
@@ -16523,7 +16828,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF32A12-AAF2-48E0-97F9-88A8DE2E9F80}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563B4475-C4FE-4C87-8240-D1D3FF54E0A4}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16769,13 +17074,13 @@
       <c r="E5" s="67" t="s">
         <v>167</v>
       </c>
-      <c r="F5" s="67" t="s">
+      <c r="F5" s="46" t="s">
         <v>1205</v>
       </c>
       <c r="G5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="67" t="s">
+      <c r="H5" s="46" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="67" t="s">
@@ -16784,7 +17089,7 @@
       <c r="J5" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="K5" s="67" t="s">
+      <c r="K5" s="46" t="s">
         <v>1253</v>
       </c>
       <c r="L5" s="67" t="s">
@@ -16796,7 +17101,7 @@
       <c r="N5" s="67" t="s">
         <v>164</v>
       </c>
-      <c r="O5" s="67" t="s">
+      <c r="O5" s="46" t="s">
         <v>23</v>
       </c>
       <c r="P5" s="67" t="s">
@@ -16943,7 +17248,7 @@
       <c r="D9" s="67" t="s">
         <v>199</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="46" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="67" t="s">
@@ -16952,34 +17257,34 @@
       <c r="G9" s="67" t="s">
         <v>185</v>
       </c>
-      <c r="H9" s="67" t="s">
+      <c r="H9" s="46" t="s">
         <v>259</v>
       </c>
       <c r="I9" s="67" t="s">
         <v>1241</v>
       </c>
-      <c r="J9" s="67" t="s">
+      <c r="J9" s="46" t="s">
         <v>1242</v>
       </c>
-      <c r="K9" s="67" t="s">
+      <c r="K9" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="67" t="s">
+      <c r="L9" s="46" t="s">
         <v>1156</v>
       </c>
       <c r="M9" s="67" t="s">
         <v>1198</v>
       </c>
-      <c r="N9" s="67" t="s">
+      <c r="N9" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="O9" s="67" t="s">
+      <c r="O9" s="46" t="s">
         <v>1202</v>
       </c>
-      <c r="P9" s="67" t="s">
+      <c r="P9" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" s="67" t="s">
+      <c r="Q9" s="46" t="s">
         <v>1209</v>
       </c>
       <c r="R9" s="67" t="s">
@@ -17092,29 +17397,31 @@
         <f>B9+1</f>
         <v>3</v>
       </c>
-      <c r="D13" s="67" t="s">
+      <c r="D13" s="46" t="s">
         <v>1158</v>
       </c>
       <c r="E13" s="67" t="s">
         <v>1248</v>
       </c>
-      <c r="F13" s="67" t="s">
+      <c r="F13" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="67" t="s">
+      <c r="G13" s="46" t="s">
         <v>1233</v>
       </c>
       <c r="H13" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="I13" s="67" t="s">
+      <c r="I13" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="J13" s="67" t="s">
+      <c r="J13" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="67" t="s">
-        <v>1478</v>
+      <c r="K13" s="46" t="str">
+        <f>CHAR(10)</f>
+        <v xml:space="preserve">
+</v>
       </c>
       <c r="L13" s="41"/>
       <c r="M13" s="41"/>
@@ -17201,7 +17508,7 @@
         <f>B13+1</f>
         <v>4</v>
       </c>
-      <c r="D17" s="67" t="str">
+      <c r="D17" s="46" t="str">
         <f>CHAR(10)</f>
         <v xml:space="preserve">
 </v>
@@ -17320,46 +17627,46 @@
         <f>B17+1</f>
         <v>5</v>
       </c>
-      <c r="D21" s="67" t="s">
+      <c r="D21" s="46" t="s">
         <v>1245</v>
       </c>
-      <c r="E21" s="67" t="s">
+      <c r="E21" s="46" t="s">
         <v>1203</v>
       </c>
-      <c r="F21" s="67" t="s">
+      <c r="F21" s="46" t="s">
         <v>1360</v>
       </c>
-      <c r="G21" s="67" t="s">
+      <c r="G21" s="46" t="s">
         <v>1186</v>
       </c>
       <c r="H21" s="67" t="s">
         <v>1175</v>
       </c>
-      <c r="I21" s="67" t="s">
+      <c r="I21" s="46" t="s">
         <v>1196</v>
       </c>
-      <c r="J21" s="67" t="s">
+      <c r="J21" s="46" t="s">
         <v>1200</v>
       </c>
-      <c r="K21" s="67" t="s">
+      <c r="K21" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L21" s="67" t="s">
+      <c r="L21" s="46" t="s">
         <v>252</v>
       </c>
       <c r="M21" s="68" t="s">
         <v>1221</v>
       </c>
-      <c r="N21" s="67" t="s">
+      <c r="N21" s="46" t="s">
         <v>1218</v>
       </c>
-      <c r="O21" s="67" t="s">
+      <c r="O21" s="46" t="s">
         <v>194</v>
       </c>
-      <c r="P21" s="67" t="s">
+      <c r="P21" s="46" t="s">
         <v>1364</v>
       </c>
-      <c r="Q21" s="67" t="s">
+      <c r="Q21" s="46" t="s">
         <v>1239</v>
       </c>
       <c r="R21" s="67" t="s">
@@ -17461,10 +17768,10 @@
         <f>B21+1</f>
         <v>6</v>
       </c>
-      <c r="D25" s="67" t="s">
+      <c r="D25" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="67" t="str">
+      <c r="E25" s="46" t="str">
         <f>CHAR(10)</f>
         <v xml:space="preserve">
 </v>
@@ -17558,7 +17865,7 @@
         <f>B25+1</f>
         <v>7</v>
       </c>
-      <c r="D29" s="67" t="str">
+      <c r="D29" s="46" t="str">
         <f>CHAR(10)</f>
         <v xml:space="preserve">
 </v>
@@ -17689,46 +17996,46 @@
         <f>B29+1</f>
         <v>8</v>
       </c>
-      <c r="D33" s="67" t="s">
+      <c r="D33" s="46" t="s">
         <v>1215</v>
       </c>
-      <c r="E33" s="67" t="s">
+      <c r="E33" s="46" t="s">
         <v>1223</v>
       </c>
-      <c r="F33" s="67" t="s">
+      <c r="F33" s="46" t="s">
         <v>1180</v>
       </c>
-      <c r="G33" s="67" t="s">
+      <c r="G33" s="46" t="s">
         <v>1197</v>
       </c>
-      <c r="H33" s="67" t="s">
+      <c r="H33" s="46" t="s">
         <v>1255</v>
       </c>
-      <c r="I33" s="67" t="s">
+      <c r="I33" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="J33" s="67" t="s">
+      <c r="J33" s="46" t="s">
         <v>1193</v>
       </c>
-      <c r="K33" s="67" t="s">
+      <c r="K33" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L33" s="67" t="s">
+      <c r="L33" s="46" t="s">
         <v>298</v>
       </c>
-      <c r="M33" s="67" t="s">
+      <c r="M33" s="46" t="s">
         <v>1185</v>
       </c>
-      <c r="N33" s="67" t="s">
+      <c r="N33" s="46" t="s">
         <v>161</v>
       </c>
-      <c r="O33" s="67" t="s">
+      <c r="O33" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="P33" s="67" t="s">
+      <c r="P33" s="46" t="s">
         <v>1254</v>
       </c>
-      <c r="Q33" s="67" t="s">
+      <c r="Q33" s="46" t="s">
         <v>237</v>
       </c>
       <c r="R33" s="67" t="s">
@@ -17834,19 +18141,19 @@
         <f>B33+1</f>
         <v>9</v>
       </c>
-      <c r="D37" s="67" t="s">
+      <c r="D37" s="46" t="s">
         <v>1212</v>
       </c>
-      <c r="E37" s="67" t="s">
+      <c r="E37" s="46" t="s">
         <v>1162</v>
       </c>
-      <c r="F37" s="67" t="s">
+      <c r="F37" s="46" t="s">
         <v>1159</v>
       </c>
-      <c r="G37" s="67" t="s">
+      <c r="G37" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="H37" s="67" t="str">
+      <c r="H37" s="46" t="str">
         <f>CHAR(10)</f>
         <v xml:space="preserve">
 </v>
@@ -17941,7 +18248,7 @@
         <f>B37+1</f>
         <v>10</v>
       </c>
-      <c r="D41" s="67" t="str">
+      <c r="D41" s="46" t="str">
         <f>CHAR(10)</f>
         <v xml:space="preserve">
 </v>
@@ -18054,49 +18361,49 @@
         <f>B41+1</f>
         <v>11</v>
       </c>
-      <c r="D45" s="67" t="s">
+      <c r="D45" s="46" t="s">
         <v>1191</v>
       </c>
-      <c r="E45" s="67" t="s">
+      <c r="E45" s="46" t="s">
         <v>1190</v>
       </c>
-      <c r="F45" s="67" t="s">
+      <c r="F45" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="G45" s="67" t="s">
+      <c r="G45" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="H45" s="67" t="s">
+      <c r="H45" s="46" t="s">
         <v>1220</v>
       </c>
-      <c r="I45" s="67" t="s">
+      <c r="I45" s="46" t="s">
         <v>262</v>
       </c>
-      <c r="J45" s="67" t="s">
+      <c r="J45" s="46" t="s">
         <v>1257</v>
       </c>
-      <c r="K45" s="67" t="s">
+      <c r="K45" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L45" s="67" t="s">
+      <c r="L45" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="M45" s="67" t="s">
+      <c r="M45" s="46" t="s">
         <v>1217</v>
       </c>
-      <c r="N45" s="67" t="s">
+      <c r="N45" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="O45" s="67" t="s">
+      <c r="O45" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="P45" s="67" t="s">
+      <c r="P45" s="46" t="s">
         <v>1199</v>
       </c>
-      <c r="Q45" s="67" t="s">
+      <c r="Q45" s="46" t="s">
         <v>1244</v>
       </c>
-      <c r="R45" s="67" t="s">
+      <c r="R45" s="46" t="s">
         <v>1195</v>
       </c>
       <c r="S45" s="21"/>
@@ -18199,19 +18506,19 @@
         <f>B45+1</f>
         <v>12</v>
       </c>
-      <c r="D49" s="67" t="s">
+      <c r="D49" s="46" t="s">
         <v>1231</v>
       </c>
-      <c r="E49" s="67" t="s">
+      <c r="E49" s="46" t="s">
         <v>1189</v>
       </c>
-      <c r="F49" s="67" t="s">
+      <c r="F49" s="46" t="s">
         <v>1187</v>
       </c>
-      <c r="G49" s="67" t="s">
+      <c r="G49" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="H49" s="67" t="str">
+      <c r="H49" s="46" t="str">
         <f>CHAR(10)</f>
         <v xml:space="preserve">
 </v>
@@ -18300,7 +18607,7 @@
         <f>B49+1</f>
         <v>13</v>
       </c>
-      <c r="D53" s="67" t="str">
+      <c r="D53" s="46" t="str">
         <f>CHAR(10)</f>
         <v xml:space="preserve">
 </v>
@@ -18415,49 +18722,49 @@
         <f>B53+1</f>
         <v>14</v>
       </c>
-      <c r="D57" s="67" t="s">
+      <c r="D57" s="46" t="s">
         <v>1214</v>
       </c>
-      <c r="E57" s="67" t="s">
+      <c r="E57" s="46" t="s">
         <v>1238</v>
       </c>
-      <c r="F57" s="67" t="s">
+      <c r="F57" s="46" t="s">
         <v>1157</v>
       </c>
-      <c r="G57" s="69" t="s">
+      <c r="G57" s="61" t="s">
         <v>1182</v>
       </c>
-      <c r="H57" s="67" t="s">
+      <c r="H57" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="I57" s="67" t="s">
+      <c r="I57" s="46" t="s">
         <v>1250</v>
       </c>
-      <c r="J57" s="67" t="s">
+      <c r="J57" s="46" t="s">
         <v>280</v>
       </c>
-      <c r="K57" s="67" t="s">
+      <c r="K57" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L57" s="67" t="s">
+      <c r="L57" s="46" t="s">
         <v>299</v>
       </c>
       <c r="M57" s="67" t="s">
         <v>199</v>
       </c>
-      <c r="N57" s="67" t="s">
+      <c r="N57" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="O57" s="67" t="s">
+      <c r="O57" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="P57" s="67" t="s">
+      <c r="P57" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="Q57" s="67" t="s">
+      <c r="Q57" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="R57" s="67" t="s">
+      <c r="R57" s="46" t="s">
         <v>164</v>
       </c>
       <c r="S57" s="21"/>
@@ -18562,19 +18869,19 @@
         <f>B57+1</f>
         <v>15</v>
       </c>
-      <c r="D61" s="67" t="s">
+      <c r="D61" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="E61" s="67" t="s">
+      <c r="E61" s="46" t="s">
         <v>26</v>
       </c>
       <c r="F61" s="67" t="s">
         <v>1248</v>
       </c>
-      <c r="G61" s="69" t="s">
+      <c r="G61" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="H61" s="67" t="s">
+      <c r="H61" s="46" t="s">
         <v>38</v>
       </c>
       <c r="I61" s="41"/>

</xml_diff>